<commit_message>
list of edits to do
</commit_message>
<xml_diff>
--- a/book/book_edits.xlsx
+++ b/book/book_edits.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>caption</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>problem</t>
+  </si>
+  <si>
+    <t>GBD region names</t>
   </si>
 </sst>
 </file>
@@ -474,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,72 +545,72 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>11</v>
+      <c r="A8" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
         <v>32</v>
@@ -615,26 +618,26 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -642,7 +645,7 @@
         <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -650,20 +653,20 @@
         <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
         <v>32</v>
@@ -671,7 +674,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
         <v>32</v>
@@ -679,7 +682,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
         <v>32</v>
@@ -687,7 +690,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>32</v>
@@ -695,42 +698,42 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -738,7 +741,7 @@
         <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -746,7 +749,7 @@
         <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -754,7 +757,7 @@
         <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -762,12 +765,12 @@
         <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
         <v>32</v>
@@ -775,7 +778,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B37" t="s">
         <v>32</v>
@@ -783,20 +786,20 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>125</v>
+        <v>115</v>
+      </c>
+      <c r="B38" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>126</v>
-      </c>
-      <c r="B39" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B40" t="s">
         <v>32</v>
@@ -804,23 +807,23 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B43" t="s">
         <v>32</v>
@@ -828,10 +831,10 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -839,71 +842,71 @@
         <v>148</v>
       </c>
       <c r="B45" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="B48" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B49" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B51" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B52" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B53" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -911,47 +914,47 @@
         <v>199</v>
       </c>
       <c r="B54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B55" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B56" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B57" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B59" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -959,7 +962,7 @@
         <v>229</v>
       </c>
       <c r="B60" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -967,7 +970,7 @@
         <v>229</v>
       </c>
       <c r="B61" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -980,17 +983,25 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B63" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
+        <v>236</v>
+      </c>
+      <c r="B64" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
         <v>240</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
book: Chris edits to intro
</commit_message>
<xml_diff>
--- a/book/book_edits.xlsx
+++ b/book/book_edits.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="315" windowWidth="18915" windowHeight="7965"/>
+    <workbookView xWindow="480" yWindow="315" windowWidth="18915" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="copy editor" sheetId="1" r:id="rId1"/>
+    <sheet name="Chris" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
   <si>
     <t>caption</t>
   </si>
@@ -124,6 +124,60 @@
   </si>
   <si>
     <t>GBD region names</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>pre….. ? Risk …s not YLDs</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>diverse</t>
+  </si>
+  <si>
+    <t>use of word novel</t>
+  </si>
+  <si>
+    <t>citation for YLD paper</t>
+  </si>
+  <si>
+    <t>many …. TV …. This</t>
+  </si>
+  <si>
+    <t>… data are not for these years</t>
+  </si>
+  <si>
+    <t>define pure number</t>
+  </si>
+  <si>
+    <t>figure</t>
+  </si>
+  <si>
+    <t>why do we allow for 1990 data … 1980 but not for 2010</t>
+  </si>
+  <si>
+    <t>country level fixed effects</t>
+  </si>
+  <si>
+    <t>figure scale</t>
+  </si>
+  <si>
+    <t>wording strange "might be"</t>
+  </si>
+  <si>
+    <t>why give statistics of ACS and AMS?</t>
+  </si>
+  <si>
+    <t>not correct, prosanto made this. DisMod1. this is not correct.</t>
+  </si>
+  <si>
+    <t>Lotus ref</t>
+  </si>
+  <si>
+    <t>number of national burden of disease studies</t>
   </si>
 </sst>
 </file>
@@ -167,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -176,6 +230,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1016,12 +1073,179 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="4">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="4">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="4">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="4">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="4">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="4">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="4">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="4">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="4">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="4">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="4">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="4">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="4">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="4">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="4">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="4">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
book: Chris edits part II
</commit_message>
<xml_diff>
--- a/book/book_edits.xlsx
+++ b/book/book_edits.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="106">
   <si>
     <t>caption</t>
   </si>
@@ -178,6 +178,162 @@
   </si>
   <si>
     <t>number of national burden of disease studies</t>
+  </si>
+  <si>
+    <t>there are no accepted definitions unnecessary</t>
+  </si>
+  <si>
+    <t>figure/text x-axis label</t>
+  </si>
+  <si>
+    <t>unnecessary, all modles are not necessarily wrong</t>
+  </si>
+  <si>
+    <t>the problem is much begger! It can lead to massive bias not just too small Uis (fig 2.1)</t>
+  </si>
+  <si>
+    <t>figure, bias not just too cor….</t>
+  </si>
+  <si>
+    <t>something very odd … …beta-binomial is unbiased but binomis is …?</t>
+  </si>
+  <si>
+    <t>prevalence cannot be greater than 1</t>
+  </si>
+  <si>
+    <t>figure-why no Uis so much wider than beta-binomial</t>
+  </si>
+  <si>
+    <t>more …. Can you show p…rs</t>
+  </si>
+  <si>
+    <t>?NSV low FITS in?</t>
+  </si>
+  <si>
+    <t>why would this be ….? No a byesion view</t>
+  </si>
+  <si>
+    <t>clarity of sentence issue</t>
+  </si>
+  <si>
+    <t>table shows offset lognormal is better</t>
+  </si>
+  <si>
+    <t>reword text</t>
+  </si>
+  <si>
+    <t>pa… if B..on lit … prior un… or … come from</t>
+  </si>
+  <si>
+    <t>figure-very … to see data from fxns</t>
+  </si>
+  <si>
+    <t>what does carefully chosen mean?</t>
+  </si>
+  <si>
+    <t>from where?</t>
+  </si>
+  <si>
+    <t>undecipherable comment</t>
+  </si>
+  <si>
+    <t>math-has clip been defined yet?</t>
+  </si>
+  <si>
+    <t>notation has not been introduced</t>
+  </si>
+  <si>
+    <t>(another) new notation</t>
+  </si>
+  <si>
+    <t>good philosophy, but in dismod you always … priors on homo….</t>
+  </si>
+  <si>
+    <t>wording sound like all non-convergence is from inconsistency</t>
+  </si>
+  <si>
+    <t>use of first person is jarring for s…. And lower. It is unnecessary you are not stating an opinion</t>
+  </si>
+  <si>
+    <t>I am not sure you are right. Intervals .. In … data</t>
+  </si>
+  <si>
+    <t>integrating … over … range sounds … and it this a bit belabored?</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>that</t>
+  </si>
+  <si>
+    <t>this does not actually … a far … as disaggreation. … assumpion is a universal … you assume anyway</t>
+  </si>
+  <si>
+    <t>tabel units? … so small?</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>this refers to using fixed and random. I think you are misusing the term</t>
+  </si>
+  <si>
+    <t>you are not yet (?) addressing the … issue of disdinguishing Res from gamma in neg binomial</t>
+  </si>
+  <si>
+    <t>why? This is not ... why you impose this</t>
+  </si>
+  <si>
+    <t>meaning what in dismod-me? Res are …</t>
+  </si>
+  <si>
+    <t>math-not true</t>
+  </si>
+  <si>
+    <t>math-notation implies constant …</t>
+  </si>
+  <si>
+    <t>math-only would inform … on … very odd</t>
+  </si>
+  <si>
+    <t>figure-what is S i C</t>
+  </si>
+  <si>
+    <t>My</t>
+  </si>
+  <si>
+    <t>figure whitespace in ball</t>
+  </si>
+  <si>
+    <t>What is … in this part? Seems like a lot of overhead on MCMC and Gibbs sampling</t>
+  </si>
+  <si>
+    <t>figure-where are …. Knots? Whey … not show up in …?</t>
+  </si>
+  <si>
+    <t>how do you choose? The … suggest age patterns in …</t>
+  </si>
+  <si>
+    <t>why sensitivity analysis? To demonstrate robust is strictly arbitray? Need to explay why this is useful</t>
+  </si>
+  <si>
+    <t>none of .. Are .. If … you … for disont… of onset. You need to discuss interaction … and setting p(a)=0</t>
+  </si>
+  <si>
+    <t>I have no idea what this chapter is saying</t>
+  </si>
+  <si>
+    <t>bigger limitation is assuming consi… over ages and sexes</t>
+  </si>
+  <si>
+    <t>wrong wording-FE are always at the country level</t>
+  </si>
+  <si>
+    <t>what is the right approach for analysis?</t>
+  </si>
+  <si>
+    <t>for setting out the … agenda this is a bit …</t>
   </si>
 </sst>
 </file>
@@ -201,12 +357,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -221,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -231,6 +393,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1073,22 +1238,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
       <c r="B1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
       <c r="B2" s="4">
         <v>14</v>
       </c>
@@ -1108,7 +1274,6 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
       <c r="B4" s="4">
         <v>16</v>
       </c>
@@ -1117,7 +1282,6 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
       <c r="B5" s="4">
         <v>17</v>
       </c>
@@ -1126,7 +1290,6 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
       <c r="B6" s="4">
         <v>17</v>
       </c>
@@ -1135,7 +1298,6 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
       <c r="B7" s="4">
         <v>17</v>
       </c>
@@ -1144,7 +1306,6 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
       <c r="B8" s="4">
         <v>17</v>
       </c>
@@ -1164,7 +1325,6 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
       <c r="B10" s="4">
         <v>18</v>
       </c>
@@ -1206,7 +1366,6 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
       <c r="B14" s="4">
         <v>21</v>
       </c>
@@ -1215,7 +1374,6 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
       <c r="B15" s="4">
         <v>24</v>
       </c>
@@ -1243,6 +1401,492 @@
       </c>
       <c r="C17" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="4">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="4">
+        <v>47</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="4">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
+        <v>49</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
+        <v>49</v>
+      </c>
+      <c r="C31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="4">
+        <v>49</v>
+      </c>
+      <c r="C32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
+        <v>55</v>
+      </c>
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="4">
+        <v>56</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="4">
+        <v>56</v>
+      </c>
+      <c r="C35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="4">
+        <v>57</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="4">
+        <v>57</v>
+      </c>
+      <c r="C37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="4">
+        <v>62</v>
+      </c>
+      <c r="C38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="4">
+        <v>63</v>
+      </c>
+      <c r="C39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="4">
+        <v>63</v>
+      </c>
+      <c r="C40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="4">
+        <v>63</v>
+      </c>
+      <c r="C41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="4">
+        <v>63</v>
+      </c>
+      <c r="C42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="4">
+        <v>65</v>
+      </c>
+      <c r="C43" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="4">
+        <v>66</v>
+      </c>
+      <c r="C44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="4">
+        <v>67</v>
+      </c>
+      <c r="C45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="4">
+        <v>68</v>
+      </c>
+      <c r="C46" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" s="4">
+        <v>69</v>
+      </c>
+      <c r="C47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="4">
+        <v>70</v>
+      </c>
+      <c r="C48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="4">
+        <v>77</v>
+      </c>
+      <c r="C49" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" s="4">
+        <v>79</v>
+      </c>
+      <c r="C50" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="4">
+        <v>79</v>
+      </c>
+      <c r="C51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="4">
+        <v>80</v>
+      </c>
+      <c r="C52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="4">
+        <v>87</v>
+      </c>
+      <c r="C53" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="4">
+        <v>88</v>
+      </c>
+      <c r="C54" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="4">
+        <v>91</v>
+      </c>
+      <c r="C55" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="4">
+        <v>91</v>
+      </c>
+      <c r="C56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="4">
+        <v>91</v>
+      </c>
+      <c r="C57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" s="4">
+        <v>96</v>
+      </c>
+      <c r="C58" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59" s="4">
+        <v>97</v>
+      </c>
+      <c r="C59" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="5">
+        <v>100</v>
+      </c>
+      <c r="C60" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" s="4">
+        <v>102</v>
+      </c>
+      <c r="C61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" s="4">
+        <v>102</v>
+      </c>
+      <c r="C62" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" s="4">
+        <v>103</v>
+      </c>
+      <c r="C63" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="4">
+        <v>104</v>
+      </c>
+      <c r="C64" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="4">
+        <v>111</v>
+      </c>
+      <c r="C65" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="4">
+        <v>118</v>
+      </c>
+      <c r="C66" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="4">
+        <v>118</v>
+      </c>
+      <c r="C67" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="5">
+        <v>122</v>
+      </c>
+      <c r="C68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="4">
+        <v>123</v>
+      </c>
+      <c r="C69" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="4">
+        <v>129</v>
+      </c>
+      <c r="C70" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="4">
+        <v>146</v>
+      </c>
+      <c r="C71" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B72" s="4">
+        <v>149</v>
+      </c>
+      <c r="C72" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B73" s="4">
+        <v>167</v>
+      </c>
+      <c r="C73" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="4">
+        <v>180</v>
+      </c>
+      <c r="C74" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
book: more of Chris comments
</commit_message>
<xml_diff>
--- a/book/book_edits.xlsx
+++ b/book/book_edits.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
   <si>
     <t>caption</t>
   </si>
@@ -222,9 +222,6 @@
     <t>reword text</t>
   </si>
   <si>
-    <t>pa… if B..on lit … prior un… or … come from</t>
-  </si>
-  <si>
     <t>figure-very … to see data from fxns</t>
   </si>
   <si>
@@ -237,9 +234,6 @@
     <t>undecipherable comment</t>
   </si>
   <si>
-    <t>math-has clip been defined yet?</t>
-  </si>
-  <si>
     <t>notation has not been introduced</t>
   </si>
   <si>
@@ -303,24 +297,15 @@
     <t>My</t>
   </si>
   <si>
-    <t>figure whitespace in ball</t>
-  </si>
-  <si>
     <t>What is … in this part? Seems like a lot of overhead on MCMC and Gibbs sampling</t>
   </si>
   <si>
     <t>figure-where are …. Knots? Whey … not show up in …?</t>
   </si>
   <si>
-    <t>how do you choose? The … suggest age patterns in …</t>
-  </si>
-  <si>
     <t>why sensitivity analysis? To demonstrate robust is strictly arbitray? Need to explay why this is useful</t>
   </si>
   <si>
-    <t>none of .. Are .. If … you … for disont… of onset. You need to discuss interaction … and setting p(a)=0</t>
-  </si>
-  <si>
     <t>I have no idea what this chapter is saying</t>
   </si>
   <si>
@@ -334,6 +319,21 @@
   </si>
   <si>
     <t>for setting out the … agenda this is a bit …</t>
+  </si>
+  <si>
+    <t>none of these are plausible! If … you … for disont… of onset. You need to discuss interaction … and setting p(a)=0</t>
+  </si>
+  <si>
+    <t>how do you choose? The figure suggest age patterns in arbitrary</t>
+  </si>
+  <si>
+    <t>figure whitespace in ball, if flak, add more points</t>
+  </si>
+  <si>
+    <t>math-has clip been defined yet?, YES</t>
+  </si>
+  <si>
+    <t>paramount if based on lit then that would be in the model. ... prior un… or … come from,</t>
   </si>
 </sst>
 </file>
@@ -357,7 +357,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,6 +367,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -383,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -396,6 +402,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1240,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,11 +1539,14 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B33" s="4">
         <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1539,7 +1554,7 @@
         <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1547,7 +1562,7 @@
         <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1555,7 +1570,7 @@
         <v>57</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1563,31 +1578,40 @@
         <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B38" s="4">
         <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B39" s="4">
         <v>63</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B40" s="4">
         <v>63</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1595,7 +1619,7 @@
         <v>63</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1603,7 +1627,7 @@
         <v>63</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1614,7 +1638,7 @@
         <v>65</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1622,7 +1646,7 @@
         <v>66</v>
       </c>
       <c r="C44" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1630,7 +1654,7 @@
         <v>67</v>
       </c>
       <c r="C45" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1638,7 +1662,7 @@
         <v>68</v>
       </c>
       <c r="C46" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1649,7 +1673,7 @@
         <v>69</v>
       </c>
       <c r="C47" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1657,7 +1681,7 @@
         <v>70</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1665,7 +1689,7 @@
         <v>77</v>
       </c>
       <c r="C49" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1676,7 +1700,7 @@
         <v>79</v>
       </c>
       <c r="C50" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1684,7 +1708,7 @@
         <v>79</v>
       </c>
       <c r="C51" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1692,7 +1716,7 @@
         <v>80</v>
       </c>
       <c r="C52" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1700,7 +1724,7 @@
         <v>87</v>
       </c>
       <c r="C53" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1708,31 +1732,31 @@
         <v>88</v>
       </c>
       <c r="C54" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="7">
+        <v>91</v>
+      </c>
+      <c r="C55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="7">
+        <v>91</v>
+      </c>
+      <c r="C56" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="4">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="7">
         <v>91</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C57" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="4">
-        <v>91</v>
-      </c>
-      <c r="C56" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="4">
-        <v>91</v>
-      </c>
-      <c r="C57" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1743,7 +1767,7 @@
         <v>96</v>
       </c>
       <c r="C58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1754,7 +1778,7 @@
         <v>97</v>
       </c>
       <c r="C59" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1762,7 +1786,7 @@
         <v>100</v>
       </c>
       <c r="C60" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1773,7 +1797,7 @@
         <v>102</v>
       </c>
       <c r="C61" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1784,7 +1808,7 @@
         <v>102</v>
       </c>
       <c r="C62" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1795,15 +1819,18 @@
         <v>103</v>
       </c>
       <c r="C63" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B64" s="4">
         <v>104</v>
       </c>
       <c r="C64" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1811,39 +1838,51 @@
         <v>111</v>
       </c>
       <c r="C65" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B66" s="4">
         <v>118</v>
       </c>
       <c r="C66" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B67" s="4">
         <v>118</v>
       </c>
       <c r="C67" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="5">
+      <c r="A68" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68" s="6">
         <v>122</v>
       </c>
       <c r="C68" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B69" s="4">
         <v>123</v>
       </c>
       <c r="C69" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1851,15 +1890,18 @@
         <v>129</v>
       </c>
       <c r="C70" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B71" s="4">
         <v>146</v>
       </c>
       <c r="C71" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1870,15 +1912,18 @@
         <v>149</v>
       </c>
       <c r="C72" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B73" s="4">
         <v>167</v>
       </c>
       <c r="C73" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1886,7 +1931,7 @@
         <v>180</v>
       </c>
       <c r="C74" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
book: more Chris edits
</commit_message>
<xml_diff>
--- a/book/book_edits.xlsx
+++ b/book/book_edits.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="108">
   <si>
     <t>caption</t>
   </si>
@@ -144,9 +144,6 @@
     <t>citation for YLD paper</t>
   </si>
   <si>
-    <t>many …. TV …. This</t>
-  </si>
-  <si>
     <t>… data are not for these years</t>
   </si>
   <si>
@@ -204,12 +201,6 @@
     <t>figure-why no Uis so much wider than beta-binomial</t>
   </si>
   <si>
-    <t>more …. Can you show p…rs</t>
-  </si>
-  <si>
-    <t>?NSV low FITS in?</t>
-  </si>
-  <si>
     <t>why would this be ….? No a byesion view</t>
   </si>
   <si>
@@ -231,39 +222,24 @@
     <t>from where?</t>
   </si>
   <si>
-    <t>undecipherable comment</t>
-  </si>
-  <si>
     <t>notation has not been introduced</t>
   </si>
   <si>
     <t>(another) new notation</t>
   </si>
   <si>
-    <t>good philosophy, but in dismod you always … priors on homo….</t>
-  </si>
-  <si>
     <t>wording sound like all non-convergence is from inconsistency</t>
   </si>
   <si>
     <t>use of first person is jarring for s…. And lower. It is unnecessary you are not stating an opinion</t>
   </si>
   <si>
-    <t>I am not sure you are right. Intervals .. In … data</t>
-  </si>
-  <si>
-    <t>integrating … over … range sounds … and it this a bit belabored?</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
     <t>that</t>
   </si>
   <si>
-    <t>this does not actually … a far … as disaggreation. … assumpion is a universal … you assume anyway</t>
-  </si>
-  <si>
     <t>tabel units? … so small?</t>
   </si>
   <si>
@@ -273,15 +249,6 @@
     <t>this refers to using fixed and random. I think you are misusing the term</t>
   </si>
   <si>
-    <t>you are not yet (?) addressing the … issue of disdinguishing Res from gamma in neg binomial</t>
-  </si>
-  <si>
-    <t>why? This is not ... why you impose this</t>
-  </si>
-  <si>
-    <t>meaning what in dismod-me? Res are …</t>
-  </si>
-  <si>
     <t>math-not true</t>
   </si>
   <si>
@@ -297,9 +264,6 @@
     <t>My</t>
   </si>
   <si>
-    <t>What is … in this part? Seems like a lot of overhead on MCMC and Gibbs sampling</t>
-  </si>
-  <si>
     <t>figure-where are …. Knots? Whey … not show up in …?</t>
   </si>
   <si>
@@ -318,9 +282,6 @@
     <t>what is the right approach for analysis?</t>
   </si>
   <si>
-    <t>for setting out the … agenda this is a bit …</t>
-  </si>
-  <si>
     <t>none of these are plausible! If … you … for disont… of onset. You need to discuss interaction … and setting p(a)=0</t>
   </si>
   <si>
@@ -334,6 +295,51 @@
   </si>
   <si>
     <t>paramount if based on lit then that would be in the model. ... prior un… or … come from,</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>more …. Can you show plots</t>
+  </si>
+  <si>
+    <t>?NSV how FITS in?</t>
+  </si>
+  <si>
+    <t>make schitzo table</t>
+  </si>
+  <si>
+    <t>chapter ends abruptly</t>
+  </si>
+  <si>
+    <t>good philosophy, but in dismod you always have priors on non...homo?</t>
+  </si>
+  <si>
+    <t>I am not sure you are right. Intervals are in the data</t>
+  </si>
+  <si>
+    <t>integrating likilihood over age range sounds pretty straightforward and it this a bit belabored?</t>
+  </si>
+  <si>
+    <t>this does not actually seem a fair representation of disaggreation. … assumpion is a universal … you assume anyway</t>
+  </si>
+  <si>
+    <t>you are not yet (?) addressing the key issue of disdinguishing Res from gamma in neg binomial</t>
+  </si>
+  <si>
+    <t>why? This is not really explained why you impose this</t>
+  </si>
+  <si>
+    <t>meaning what in dismod-me? Res are all set</t>
+  </si>
+  <si>
+    <t>What is original in this part? Seems like a lot of overhead on MCMC and Gibbs sampling</t>
+  </si>
+  <si>
+    <t>for setting out the research agenda this is a bit weak</t>
+  </si>
+  <si>
+    <t>may want to define this</t>
   </si>
 </sst>
 </file>
@@ -357,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -376,6 +382,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -389,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -408,6 +420,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1250,10 +1271,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,6 +1288,9 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B2" s="4">
         <v>14</v>
       </c>
@@ -1286,7 +1310,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="4">
+      <c r="B4" s="5">
         <v>16</v>
       </c>
       <c r="C4" t="s">
@@ -1306,7 +1330,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1314,15 +1338,18 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B8" s="4">
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1333,15 +1360,18 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B10" s="4">
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1352,7 +1382,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1363,7 +1393,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1374,23 +1404,27 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B14" s="4">
         <v>21</v>
       </c>
       <c r="C14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1401,7 +1435,7 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1412,31 +1446,40 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B18" s="4">
         <v>32</v>
       </c>
       <c r="C18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="10">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="4">
-        <v>33</v>
-      </c>
-      <c r="C19" t="s">
-        <v>55</v>
-      </c>
-    </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B20" s="4">
         <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1444,7 +1487,7 @@
         <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1452,7 +1495,7 @@
         <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1460,7 +1503,7 @@
         <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1471,7 +1514,7 @@
         <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1479,31 +1522,32 @@
         <v>43</v>
       </c>
       <c r="C25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="5">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="5">
+        <v>47</v>
+      </c>
+      <c r="C28" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="4">
-        <v>44</v>
-      </c>
-      <c r="C26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="4">
-        <v>46</v>
-      </c>
-      <c r="C27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="4">
-        <v>47</v>
-      </c>
-      <c r="C28" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1511,11 +1555,12 @@
         <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="4">
+      <c r="A30" s="9"/>
+      <c r="B30" s="10">
         <v>49</v>
       </c>
       <c r="C30" t="s">
@@ -1523,38 +1568,41 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="4">
+      <c r="A31" s="9"/>
+      <c r="B31" s="10">
         <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="4">
+      <c r="A32" s="9"/>
+      <c r="B32" s="10">
         <v>49</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="4">
+      <c r="A33" s="9"/>
+      <c r="B33" s="10">
+        <v>49</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="4">
         <v>55</v>
       </c>
-      <c r="C33" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="4">
-        <v>56</v>
-      </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1562,15 +1610,15 @@
         <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="4">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1578,18 +1626,16 @@
         <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="4">
-        <v>62</v>
+      <c r="A38" s="8"/>
+      <c r="B38" s="6">
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1597,10 +1643,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="4">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1611,23 +1657,26 @@
         <v>63</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B41" s="4">
         <v>63</v>
       </c>
       <c r="C41" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="4">
+      <c r="B42" s="5">
         <v>63</v>
       </c>
       <c r="C42" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1635,112 +1684,129 @@
         <v>38</v>
       </c>
       <c r="B43" s="4">
+        <v>63</v>
+      </c>
+      <c r="C43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="4">
         <v>65</v>
       </c>
-      <c r="C43" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="4">
+      <c r="C44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="4">
         <v>66</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="10">
+        <v>67</v>
+      </c>
+      <c r="C46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="5">
+        <v>68</v>
+      </c>
+      <c r="C47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="4">
+        <v>69</v>
+      </c>
+      <c r="C48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="5">
+        <v>71</v>
+      </c>
+      <c r="C49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="9"/>
+      <c r="B50" s="10">
         <v>77</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="4">
-        <v>67</v>
-      </c>
-      <c r="C45" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="4">
-        <v>68</v>
-      </c>
-      <c r="C46" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B47" s="4">
-        <v>69</v>
-      </c>
-      <c r="C47" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="4">
-        <v>70</v>
-      </c>
-      <c r="C48" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="4">
-        <v>77</v>
-      </c>
-      <c r="C49" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B50" s="4">
-        <v>79</v>
-      </c>
       <c r="C50" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B51" s="4">
         <v>79</v>
       </c>
       <c r="C51" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B52" s="4">
+        <v>79</v>
+      </c>
+      <c r="C52" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="9"/>
+      <c r="B53" s="10">
         <v>80</v>
       </c>
-      <c r="C52" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="4">
+      <c r="C53" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" s="4">
         <v>87</v>
       </c>
-      <c r="C53" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="4">
+      <c r="C54" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="4">
         <v>88</v>
       </c>
-      <c r="C54" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="7">
-        <v>91</v>
-      </c>
       <c r="C55" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1748,7 +1814,7 @@
         <v>91</v>
       </c>
       <c r="C56" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1756,18 +1822,15 @@
         <v>91</v>
       </c>
       <c r="C57" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B58" s="4">
-        <v>96</v>
+      <c r="B58" s="7">
+        <v>91</v>
       </c>
       <c r="C58" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1775,29 +1838,29 @@
         <v>38</v>
       </c>
       <c r="B59" s="4">
+        <v>96</v>
+      </c>
+      <c r="C59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" s="4">
         <v>97</v>
       </c>
-      <c r="C59" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="5">
+      <c r="C60" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="5">
         <v>100</v>
       </c>
-      <c r="C60" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B61" s="4">
-        <v>102</v>
-      </c>
       <c r="C61" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1808,7 +1871,7 @@
         <v>102</v>
       </c>
       <c r="C62" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1816,10 +1879,10 @@
         <v>38</v>
       </c>
       <c r="B63" s="4">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C63" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1827,29 +1890,29 @@
         <v>38</v>
       </c>
       <c r="B64" s="4">
+        <v>103</v>
+      </c>
+      <c r="C64" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65" s="4">
         <v>104</v>
       </c>
-      <c r="C64" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="4">
+      <c r="C65" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="4">
         <v>111</v>
       </c>
-      <c r="C65" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B66" s="4">
-        <v>118</v>
-      </c>
       <c r="C66" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1860,48 +1923,48 @@
         <v>118</v>
       </c>
       <c r="C67" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B68" s="6">
-        <v>122</v>
+      <c r="B68" s="4">
+        <v>118</v>
       </c>
       <c r="C68" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B69" s="6">
+        <v>122</v>
+      </c>
+      <c r="C69" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B70" s="4">
         <v>123</v>
       </c>
-      <c r="C69" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="4">
+      <c r="C70" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="4">
         <v>129</v>
       </c>
-      <c r="C70" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B71" s="4">
-        <v>146</v>
-      </c>
       <c r="C71" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1909,10 +1972,10 @@
         <v>38</v>
       </c>
       <c r="B72" s="4">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C72" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1920,18 +1983,29 @@
         <v>38</v>
       </c>
       <c r="B73" s="4">
+        <v>149</v>
+      </c>
+      <c r="C73" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B74" s="4">
         <v>167</v>
       </c>
-      <c r="C73" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="4">
+      <c r="C74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="5">
         <v>180</v>
       </c>
-      <c r="C74" t="s">
-        <v>100</v>
+      <c r="C75" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
book: Chris comments cont
</commit_message>
<xml_diff>
--- a/book/book_edits.xlsx
+++ b/book/book_edits.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="108">
   <si>
     <t>caption</t>
   </si>
@@ -401,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -430,6 +430,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1273,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,6 +1316,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
       <c r="B4" s="5">
         <v>16</v>
       </c>
@@ -1318,6 +1325,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B5" s="4">
         <v>17</v>
       </c>
@@ -1326,6 +1336,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B6" s="4">
         <v>17</v>
       </c>
@@ -1334,6 +1347,9 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B7" s="4">
         <v>17</v>
       </c>
@@ -1535,6 +1551,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
       <c r="B27" s="5">
         <v>46</v>
       </c>
@@ -1543,6 +1560,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
       <c r="B28" s="5">
         <v>47</v>
       </c>
@@ -1551,6 +1569,9 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B29" s="4">
         <v>48</v>
       </c>
@@ -1672,6 +1693,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
       <c r="B42" s="5">
         <v>63</v>
       </c>
@@ -1724,6 +1746,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
       <c r="B47" s="5">
         <v>68</v>
       </c>
@@ -1743,6 +1766,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="11"/>
       <c r="B49" s="5">
         <v>71</v>
       </c>
@@ -1810,6 +1834,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="12"/>
       <c r="B56" s="7">
         <v>91</v>
       </c>
@@ -1818,6 +1843,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="12"/>
       <c r="B57" s="7">
         <v>91</v>
       </c>
@@ -1826,6 +1852,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="12"/>
       <c r="B58" s="7">
         <v>91</v>
       </c>
@@ -1856,6 +1883,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="11"/>
       <c r="B61" s="5">
         <v>100</v>
       </c>
@@ -2001,6 +2029,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="11"/>
       <c r="B75" s="5">
         <v>180</v>
       </c>

</xml_diff>

<commit_message>
book: more Chris comments
</commit_message>
<xml_diff>
--- a/book/book_edits.xlsx
+++ b/book/book_edits.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="315" windowWidth="18915" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="375" windowWidth="18915" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="copy editor" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="108">
   <si>
     <t>caption</t>
   </si>
@@ -346,7 +346,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +358,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -401,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -436,6 +442,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1279,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,10 +1489,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="10">
+      <c r="A19" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="14">
         <v>33</v>
       </c>
       <c r="C19" t="s">
@@ -1499,6 +1511,9 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B21" s="4">
         <v>36</v>
       </c>
@@ -1507,6 +1522,9 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B22" s="4">
         <v>37</v>
       </c>
@@ -1936,7 +1954,8 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="4">
+      <c r="A66" s="9"/>
+      <c r="B66" s="10">
         <v>111</v>
       </c>
       <c r="C66" t="s">
@@ -1988,6 +2007,9 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B71" s="4">
         <v>129</v>
       </c>
@@ -2039,6 +2061,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
BOOK: update figures and text about spline models and expert priors
</commit_message>
<xml_diff>
--- a/book/book_edits.xlsx
+++ b/book/book_edits.xlsx
@@ -40,9 +40,6 @@
     <t>age group (n) v age-group (adj)</t>
   </si>
   <si>
-    <t>all </t>
-  </si>
-  <si>
     <t>number font</t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>reword text</t>
+  </si>
+  <si>
+    <t>needs more</t>
   </si>
   <si>
     <t>paramount if based on lit then that would be in the model. ... prior un… or … come from,</t>
@@ -466,7 +466,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -478,13 +478,10 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
@@ -499,7 +496,7 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
   </cellXfs>
@@ -526,8 +523,8 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5254901960784"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
@@ -572,18 +569,18 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
       <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
@@ -591,7 +588,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
@@ -599,7 +596,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
@@ -607,7 +604,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
@@ -615,7 +612,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
@@ -623,7 +620,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
@@ -631,7 +628,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
@@ -639,7 +636,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
@@ -647,7 +644,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
@@ -655,7 +652,7 @@
         <v>49</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
@@ -663,7 +660,7 @@
         <v>51</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
@@ -671,7 +668,7 @@
         <v>52</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
@@ -679,7 +676,7 @@
         <v>58</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
@@ -687,7 +684,7 @@
         <v>59</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
@@ -695,7 +692,7 @@
         <v>59</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22">
@@ -703,7 +700,7 @@
         <v>59</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
@@ -711,7 +708,7 @@
         <v>68</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
@@ -719,7 +716,7 @@
         <v>69</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="25">
@@ -727,7 +724,7 @@
         <v>71</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26">
@@ -735,7 +732,7 @@
         <v>78</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
@@ -743,7 +740,7 @@
         <v>80</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28">
@@ -751,7 +748,7 @@
         <v>81</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29">
@@ -759,7 +756,7 @@
         <v>88</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="30">
@@ -767,7 +764,7 @@
         <v>90</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="31">
@@ -775,7 +772,7 @@
         <v>98</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="32">
@@ -783,7 +780,7 @@
         <v>99</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="33">
@@ -791,7 +788,7 @@
         <v>99</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="34">
@@ -799,7 +796,7 @@
         <v>99</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="35">
@@ -807,7 +804,7 @@
         <v>99</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="36">
@@ -815,7 +812,7 @@
         <v>99</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="37">
@@ -823,7 +820,7 @@
         <v>113</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="38">
@@ -831,7 +828,7 @@
         <v>115</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="39">
@@ -844,7 +841,7 @@
         <v>126</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="41">
@@ -852,7 +849,7 @@
         <v>127</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="42">
@@ -860,7 +857,7 @@
         <v>139</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="43">
@@ -868,7 +865,7 @@
         <v>144</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="44">
@@ -876,7 +873,7 @@
         <v>146</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="45">
@@ -884,7 +881,7 @@
         <v>148</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="46">
@@ -892,7 +889,7 @@
         <v>148</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="47">
@@ -900,7 +897,7 @@
         <v>149</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="48">
@@ -908,7 +905,7 @@
         <v>151</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="49">
@@ -916,7 +913,7 @@
         <v>171</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="50">
@@ -924,7 +921,7 @@
         <v>178</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="51">
@@ -932,7 +929,7 @@
         <v>195</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="52">
@@ -940,7 +937,7 @@
         <v>197</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="53">
@@ -948,7 +945,7 @@
         <v>198</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="54">
@@ -956,7 +953,7 @@
         <v>199</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="55">
@@ -964,7 +961,7 @@
         <v>199</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="56">
@@ -972,7 +969,7 @@
         <v>201</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="57">
@@ -980,7 +977,7 @@
         <v>206</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="58">
@@ -988,7 +985,7 @@
         <v>216</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="59">
@@ -996,7 +993,7 @@
         <v>222</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="60">
@@ -1004,7 +1001,7 @@
         <v>229</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="61">
@@ -1012,7 +1009,7 @@
         <v>229</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="62">
@@ -1020,7 +1017,7 @@
         <v>229</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="63">
@@ -1028,7 +1025,7 @@
         <v>229</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="64">
@@ -1036,7 +1033,7 @@
         <v>236</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="65">
@@ -1044,7 +1041,7 @@
         <v>240</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1065,369 +1062,369 @@
   </sheetPr>
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B33" activeCellId="0" pane="topLeft" sqref="B33"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A19" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A37" activeCellId="0" pane="topLeft" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="9.18039215686274"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.56862745098039"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="87.9372549019608"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="9.18039215686274"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="9.22352941176471"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.60392156862745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="88.3019607843137"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="9.22352941176471"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
       <c r="B1" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
       <c r="A2" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>14</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+      <c r="A4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
-      <c r="A4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>17</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
       <c r="A6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>17</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
       <c r="A7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
       <c r="A8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
       <c r="A9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="4" t="n">
         <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
       <c r="A10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="4" t="n">
         <v>18</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
       <c r="A11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="4" t="n">
         <v>19</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
       <c r="A12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="4" t="n">
         <v>20</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="4" t="n">
         <v>21</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
       <c r="A14" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="4" t="n">
         <v>21</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7" t="n">
+        <v>24</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8" t="n">
-        <v>24</v>
-      </c>
-      <c r="C15" s="0" t="s">
+      <c r="D15" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
       <c r="A16" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="4" t="n">
         <v>24</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
       <c r="A17" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="4" t="n">
         <v>25</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
       <c r="A18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="4" t="n">
         <v>32</v>
       </c>
       <c r="C18" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
+      <c r="A19" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="9" t="n">
+        <v>33</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
-      <c r="A19" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="10" t="n">
-        <v>33</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
       <c r="A20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="4" t="n">
         <v>35</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="4" t="n">
         <v>36</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="4" t="n">
         <v>37</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+      <c r="B23" s="10" t="n">
+        <v>38</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="23">
-      <c r="B23" s="11" t="n">
-        <v>38</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24">
       <c r="A24" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="4" t="n">
         <v>40</v>
       </c>
       <c r="C24" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="25">
+      <c r="B25" s="10" t="n">
+        <v>43</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>62</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="25">
-      <c r="B25" s="11" t="n">
-        <v>43</v>
-      </c>
-      <c r="C25" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7" t="n">
+        <v>44</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>63</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8" t="n">
-        <v>44</v>
-      </c>
-      <c r="C26" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
+      <c r="A27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>46</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>64</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
-      <c r="A27" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="6" t="n">
-        <v>46</v>
-      </c>
-      <c r="C27" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28">
+      <c r="A28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>47</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28">
-      <c r="A28" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="6" t="n">
-        <v>47</v>
-      </c>
-      <c r="C28" s="0" t="s">
+      <c r="D28" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29">
       <c r="A29" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="4" t="n">
         <v>48</v>
       </c>
       <c r="C29" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="30">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7" t="n">
+        <v>49</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="31">
+      <c r="A31" s="6"/>
+      <c r="B31" s="7" t="n">
+        <v>49</v>
+      </c>
+      <c r="C31" s="0" t="s">
         <v>68</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="30">
-      <c r="A30" s="7"/>
-      <c r="B30" s="8" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="32">
+      <c r="A32" s="6"/>
+      <c r="B32" s="7" t="n">
         <v>49</v>
       </c>
-      <c r="C30" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="31">
-      <c r="A31" s="7"/>
-      <c r="B31" s="8" t="n">
+      <c r="C32" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="33">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7" t="n">
         <v>49</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="32">
-      <c r="A32" s="7"/>
-      <c r="B32" s="8" t="n">
-        <v>49</v>
-      </c>
-      <c r="C32" s="0" t="s">
+      <c r="C33" s="0" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="33">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8" t="n">
-        <v>49</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="34">
       <c r="A34" s="3" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B34" s="4" t="n">
         <v>55</v>
@@ -1437,7 +1434,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="35">
-      <c r="A35" s="12"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="4" t="n">
         <v>56</v>
       </c>
@@ -1446,7 +1443,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="36">
-      <c r="A36" s="12"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="4" t="n">
         <v>56</v>
       </c>
@@ -1455,7 +1452,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="37">
-      <c r="A37" s="12"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="4" t="n">
         <v>57</v>
       </c>
@@ -1464,8 +1461,8 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="38">
-      <c r="A38" s="12"/>
-      <c r="B38" s="6" t="n">
+      <c r="A38" s="11"/>
+      <c r="B38" s="5" t="n">
         <v>57</v>
       </c>
       <c r="C38" s="0" t="s">
@@ -1474,7 +1471,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="39">
       <c r="A39" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="4" t="n">
         <v>62</v>
@@ -1485,7 +1482,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="40">
       <c r="A40" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" s="4" t="n">
         <v>63</v>
@@ -1496,7 +1493,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="41">
       <c r="A41" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41" s="4" t="n">
         <v>63</v>
@@ -1506,10 +1503,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="42">
-      <c r="A42" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="6" t="n">
+      <c r="A42" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="5" t="n">
         <v>63</v>
       </c>
       <c r="C42" s="0" t="s">
@@ -1521,7 +1518,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="43">
       <c r="A43" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43" s="4" t="n">
         <v>63</v>
@@ -1532,7 +1529,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="44">
       <c r="A44" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" s="4" t="n">
         <v>65</v>
@@ -1543,7 +1540,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="45">
       <c r="A45" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" s="4" t="n">
         <v>66</v>
@@ -1553,10 +1550,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="46">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="8" t="n">
+      <c r="B46" s="7" t="n">
         <v>67</v>
       </c>
       <c r="C46" s="0" t="s">
@@ -1564,10 +1561,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="47">
-      <c r="A47" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B47" s="6" t="n">
+      <c r="A47" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="5" t="n">
         <v>68</v>
       </c>
       <c r="C47" s="0" t="s">
@@ -1576,7 +1573,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="48">
       <c r="A48" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B48" s="4" t="n">
         <v>69</v>
@@ -1586,10 +1583,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="49">
-      <c r="A49" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B49" s="6" t="n">
+      <c r="A49" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" s="5" t="n">
         <v>71</v>
       </c>
       <c r="C49" s="0" t="s">
@@ -1600,8 +1597,8 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="50">
-      <c r="A50" s="7"/>
-      <c r="B50" s="8" t="n">
+      <c r="A50" s="6"/>
+      <c r="B50" s="7" t="n">
         <v>77</v>
       </c>
       <c r="C50" s="0" t="s">
@@ -1610,7 +1607,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="51">
       <c r="A51" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B51" s="4" t="n">
         <v>79</v>
@@ -1621,7 +1618,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="52">
       <c r="A52" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B52" s="4" t="n">
         <v>79</v>
@@ -1631,8 +1628,8 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="53">
-      <c r="A53" s="7"/>
-      <c r="B53" s="8" t="n">
+      <c r="A53" s="6"/>
+      <c r="B53" s="7" t="n">
         <v>80</v>
       </c>
       <c r="C53" s="0" t="s">
@@ -1641,7 +1638,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="54">
       <c r="A54" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B54" s="4" t="n">
         <v>87</v>
@@ -1651,8 +1648,8 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="55">
-      <c r="A55" s="5" t="s">
-        <v>37</v>
+      <c r="A55" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="B55" s="4" t="n">
         <v>88</v>
@@ -1662,10 +1659,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="56">
-      <c r="A56" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B56" s="6" t="n">
+      <c r="A56" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56" s="5" t="n">
         <v>91</v>
       </c>
       <c r="C56" s="0" t="s">
@@ -1673,10 +1670,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="57">
-      <c r="A57" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B57" s="6" t="n">
+      <c r="A57" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" s="5" t="n">
         <v>91</v>
       </c>
       <c r="C57" s="0" t="s">
@@ -1684,10 +1681,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="58">
-      <c r="A58" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B58" s="6" t="n">
+      <c r="A58" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58" s="5" t="n">
         <v>91</v>
       </c>
       <c r="C58" s="0" t="s">
@@ -1696,7 +1693,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="59">
       <c r="A59" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B59" s="4" t="n">
         <v>96</v>
@@ -1707,7 +1704,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="60">
       <c r="A60" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B60" s="4" t="n">
         <v>97</v>
@@ -1717,10 +1714,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="61">
-      <c r="A61" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B61" s="6" t="n">
+      <c r="A61" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B61" s="5" t="n">
         <v>100</v>
       </c>
       <c r="C61" s="0" t="s">
@@ -1729,7 +1726,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="62">
       <c r="A62" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B62" s="4" t="n">
         <v>102</v>
@@ -1740,7 +1737,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="63">
       <c r="A63" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B63" s="4" t="n">
         <v>102</v>
@@ -1751,7 +1748,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="64">
       <c r="A64" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B64" s="4" t="n">
         <v>103</v>
@@ -1762,7 +1759,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="65">
       <c r="A65" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B65" s="4" t="n">
         <v>104</v>
@@ -1772,8 +1769,8 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="66">
-      <c r="A66" s="7"/>
-      <c r="B66" s="8" t="n">
+      <c r="A66" s="6"/>
+      <c r="B66" s="7" t="n">
         <v>111</v>
       </c>
       <c r="C66" s="0" t="s">
@@ -1782,7 +1779,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="67">
       <c r="A67" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B67" s="4" t="n">
         <v>118</v>
@@ -1793,7 +1790,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="68">
       <c r="A68" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B68" s="4" t="n">
         <v>118</v>
@@ -1804,9 +1801,9 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="69">
       <c r="A69" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B69" s="6" t="n">
+        <v>36</v>
+      </c>
+      <c r="B69" s="5" t="n">
         <v>122</v>
       </c>
       <c r="C69" s="0" t="s">
@@ -1815,7 +1812,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="70">
       <c r="A70" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B70" s="4" t="n">
         <v>123</v>
@@ -1826,7 +1823,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="71">
       <c r="A71" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B71" s="4" t="n">
         <v>129</v>
@@ -1837,7 +1834,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="72">
       <c r="A72" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B72" s="4" t="n">
         <v>146</v>
@@ -1848,7 +1845,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="73">
       <c r="A73" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B73" s="4" t="n">
         <v>149</v>
@@ -1859,7 +1856,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="74">
       <c r="A74" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B74" s="4" t="n">
         <v>167</v>
@@ -1869,8 +1866,8 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="75">
-      <c r="A75" s="7"/>
-      <c r="B75" s="8" t="n">
+      <c r="A75" s="6"/>
+      <c r="B75" s="7" t="n">
         <v>180</v>
       </c>
       <c r="C75" s="0" t="s">
@@ -1903,7 +1900,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
BOOK: update age group validation table
</commit_message>
<xml_diff>
--- a/book/book_edits.xlsx
+++ b/book/book_edits.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="116">
   <si>
     <t>copy editor page number</t>
   </si>
@@ -292,7 +292,13 @@
     <t>What would be a fair representation?</t>
   </si>
   <si>
+    <t>fixed</t>
+  </si>
+  <si>
     <t>tabel units? … so small?</t>
+  </si>
+  <si>
+    <t>call them percentage points (pp) since they are difference between percentages; they should be this small</t>
   </si>
   <si>
     <t>I</t>
@@ -519,7 +525,7 @@
   <dimension ref="A1:B65"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A9" activeCellId="0" pane="topLeft" sqref="A9"/>
+      <selection activeCell="A9" activeCellId="1" pane="topLeft" sqref="C54:C65 A9"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -1062,8 +1068,8 @@
   </sheetPr>
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A19" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A37" activeCellId="0" pane="topLeft" sqref="A37"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A44" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C54" activeCellId="0" pane="topLeft" sqref="C54:C65"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -1596,13 +1602,18 @@
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="50">
-      <c r="A50" s="6"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="50">
+      <c r="A50" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="B50" s="7" t="n">
         <v>77</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="51">
@@ -1613,7 +1624,7 @@
         <v>79</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="52">
@@ -1624,7 +1635,7 @@
         <v>79</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="53">
@@ -1633,7 +1644,7 @@
         <v>80</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="54">
@@ -1644,7 +1655,7 @@
         <v>87</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="55">
@@ -1655,7 +1666,7 @@
         <v>88</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="56">
@@ -1666,7 +1677,7 @@
         <v>91</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="57">
@@ -1677,7 +1688,7 @@
         <v>91</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="58">
@@ -1688,7 +1699,7 @@
         <v>91</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="59">
@@ -1699,7 +1710,7 @@
         <v>96</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="60">
@@ -1710,7 +1721,7 @@
         <v>97</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="61">
@@ -1721,7 +1732,7 @@
         <v>100</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="62">
@@ -1732,7 +1743,7 @@
         <v>102</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="63">
@@ -1743,7 +1754,7 @@
         <v>102</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="64">
@@ -1754,7 +1765,7 @@
         <v>103</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="65">
@@ -1765,7 +1776,7 @@
         <v>104</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="66">
@@ -1774,7 +1785,7 @@
         <v>111</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="67">
@@ -1785,7 +1796,7 @@
         <v>118</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="68">
@@ -1796,7 +1807,7 @@
         <v>118</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="69">
@@ -1807,7 +1818,7 @@
         <v>122</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="70">
@@ -1818,7 +1829,7 @@
         <v>123</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="71">
@@ -1829,7 +1840,7 @@
         <v>129</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="72">
@@ -1840,7 +1851,7 @@
         <v>146</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="73">
@@ -1851,7 +1862,7 @@
         <v>149</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="74">
@@ -1862,7 +1873,7 @@
         <v>167</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="75">
@@ -1871,10 +1882,10 @@
         <v>180</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1896,7 +1907,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="C54:C65 A1"/>
     </sheetView>
   </sheetViews>
   <cols>

</xml_diff>